<commit_message>
Updated wear leveling calculations
</commit_message>
<xml_diff>
--- a/timecalculation.xlsx
+++ b/timecalculation.xlsx
@@ -16,34 +16,58 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
-  <si>
-    <t>days</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>years</t>
   </si>
   <si>
-    <t>hours</t>
-  </si>
-  <si>
-    <t>writes</t>
-  </si>
-  <si>
-    <t>spread</t>
-  </si>
-  <si>
-    <t>total writes</t>
-  </si>
-  <si>
-    <t>minutes</t>
+    <t>The EEPROM memory has a specified life of 100,000 write/erase cycles</t>
+  </si>
+  <si>
+    <t>We will assume</t>
+  </si>
+  <si>
+    <t>write/erase cycles</t>
+  </si>
+  <si>
+    <t>If we want our EEPROM to live for</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>we could write</t>
+  </si>
+  <si>
+    <t>times per cell per year</t>
+  </si>
+  <si>
+    <t>times per cell per day</t>
+  </si>
+  <si>
+    <t>times per cell per hour</t>
+  </si>
+  <si>
+    <t>cells</t>
+  </si>
+  <si>
+    <t>However, if we spread a byte over</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we can write this byte </t>
+  </si>
+  <si>
+    <t>times per hour</t>
+  </si>
+  <si>
+    <t>times per minute</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,13 +75,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,8 +118,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,95 +485,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="D1">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <f>365*D1</f>
-        <v>14600</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <f>A2*24</f>
-        <v>350400</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <f>A3*60</f>
-        <v>21024000</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>100000</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6">
+      <c r="B5" s="2">
+        <f>B3/B4</f>
+        <v>2500</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <f>B5/365</f>
+        <v>6.8493150684931505</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <f>B6/24</f>
+        <v>0.28538812785388129</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
         <v>200</v>
       </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <f>A6*D6</f>
-        <v>20000000</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3">
+        <f>B7*B9</f>
+        <v>57.077625570776256</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <f>A4/A7</f>
-        <v>1.0511999999999999</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <f>A8/60</f>
-        <v>1.7519999999999997E-2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
+      <c r="B11" s="3">
+        <f>B10/60</f>
+        <v>0.9512937595129376</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>